<commit_message>
Add remaining ICDC pages and locators
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/ICDC_StaticData.xlsx
+++ b/InputFiles/ICDC/ICDC_StaticData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EB2E47-A182-AC40-9236-DABA5A1A095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44254749-EC33-5A47-8498-A77C24D2EF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3600" windowWidth="33260" windowHeight="18380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="2060" windowWidth="33260" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="V_DataSubmissionPage" sheetId="16" r:id="rId4"/>
     <sheet name="V_ResourcesDeveloperPage" sheetId="14" r:id="rId5"/>
     <sheet name="V_AboutPurposePage" sheetId="7" r:id="rId6"/>
-    <sheet name="V_AboutCommitteePage" sheetId="8" r:id="rId7"/>
-    <sheet name="V_AboutGovernancePage" sheetId="9" r:id="rId8"/>
-    <sheet name="V_AboutBestPracticesPage" sheetId="10" r:id="rId9"/>
+    <sheet name="V_AboutSteeringPage" sheetId="8" r:id="rId7"/>
+    <sheet name="V_AboutDGABPage" sheetId="9" r:id="rId8"/>
+    <sheet name="V_AboutBPSCPage" sheetId="10" r:id="rId9"/>
     <sheet name="V_AboutWorkGroupsPage" sheetId="11" r:id="rId10"/>
     <sheet name="V_AboutCRDCPage" sheetId="12" r:id="rId11"/>
     <sheet name="V_AboutSupportPage" sheetId="13" r:id="rId12"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="281">
   <si>
     <t>verificationText</t>
   </si>
@@ -348,9 +348,6 @@
     <t>SubmissionsDescription3</t>
   </si>
   <si>
-    <t>The Integrated Canine Data Commons (ICDC) was established to further research on human cancers by enabling comparative analysis with canine malignancies. Researchers who have data that will contribute to this mission and who are willing to share that data via the ICDC are encouraged to make a data submission request through the Submission Request Process [PDF]. Please email ICDCHelpDesk@mail.nih.gov for specific instructions. All proposed data submissions are reviewed by the Data Governance Advisory Board (DGAB)outbounnd web site icon to assess their scientific value and suitability for inclusion. Once any given study has been fully on-boarded, all data submitted will become publicly available.</t>
-  </si>
-  <si>
     <t>To initiate a Data Submission Request, please use this Template</t>
   </si>
   <si>
@@ -366,9 +363,6 @@
     <t>The Data Model Navigator and Data Preparation</t>
   </si>
   <si>
-    <t>In support of data submissions, the ICDC application now includes a sophisticated and intuitive Data Model Navigatoroutbounnd web site icon which provides end users in general, and data submitters in particular, with access to a wealth of information regarding the graph-based data model upon which the ICDC is based.</t>
-  </si>
-  <si>
     <t>NavigatorDescription2</t>
   </si>
   <si>
@@ -408,12 +402,6 @@
     <t>Developers</t>
   </si>
   <si>
-    <t>Description1</t>
-  </si>
-  <si>
-    <t>Description2</t>
-  </si>
-  <si>
     <t>https://caninecommons.cancer.gov/v1/graphql/</t>
   </si>
   <si>
@@ -423,9 +411,6 @@
     <t>GithubTitle</t>
   </si>
   <si>
-    <t>GithubDescription1</t>
-  </si>
-  <si>
     <t>GraphqlLink</t>
   </si>
   <si>
@@ -483,30 +468,12 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Purpose_BannerTitle</t>
-  </si>
-  <si>
-    <t>Purpose_Description1</t>
-  </si>
-  <si>
-    <t>NCI's Division of Cancer Treatment and Diagnosis (DCTD) tasked the Frederick National Laboratory for Cancer Research (FNLCR) with building the Integrated Canine Data Commons (ICDC), a cloud-based repository of spontaneously-arising canine cancer data. ICDC was established to further research on human cancers by enabling comparative analysis with canine cancer. The data in the ICDC is sourced from multiple different programs and projects; all focused on canine subjects. The data is harmonized into an integrated data model and then made available to the research community. The ICDC is part of the Cancer Research Data Commons (CRDC)outbounnd web site icon, an initiative from NCI’s Center for Biomedical Informatics and Information Technology (CBIIT). Bioinformatic analysis of the ICDC data is accomplished using the CRDC’s Cloud Resources.</t>
-  </si>
-  <si>
     <t>The FNLCR Bioinformatics and Computational Science (BACS) Directorate has a focus on software engineering and data science and is responsible for devlopment of the ICDC web application and overall management of the project and The Applied and Developmental Research Directorate (ADRD) has a focus on clinical and biological monitoring and assay development and manages the ICDC Steering Committee and provides one of the data sources for the ICDC. The ICDC Steering Committee is comprised of external members, FNLCR and NCI staff that provide guidance to DCTD on the ICDC.</t>
   </si>
   <si>
-    <t>Purpose_CrdcLink</t>
-  </si>
-  <si>
-    <t>Cancer Research Data Commons (CRDC)</t>
-  </si>
-  <si>
     <t>Cloud Resources</t>
   </si>
   <si>
-    <t>Purpose_CloudLink</t>
-  </si>
-  <si>
     <t>https://datacommons.cancer.gov/</t>
   </si>
   <si>
@@ -589,6 +556,328 @@
   </si>
   <si>
     <t>To cite an individual study, cite the native ICDC accession ID as displayed within the User Interface, prefixed by “icdc:” to create a compact identifier that can be resolved via identifiers.org (e.g., icdc:000003), and/or cite the URL to the study (e.g., https://caninecommons.cancer.gov/#/study/000003), where the URL ends with the native ICDC accession ID.</t>
+  </si>
+  <si>
+    <t>SubmissionsProcessLink</t>
+  </si>
+  <si>
+    <t>SubmissionsDGABLink</t>
+  </si>
+  <si>
+    <t>SubmissionsTemplateLink</t>
+  </si>
+  <si>
+    <t>NavigatorLink</t>
+  </si>
+  <si>
+    <t>Submission Request Process [PDF]</t>
+  </si>
+  <si>
+    <t>https://github.com/CBIIT/icdc-codebase/raw/master/src/main/frontend/src/content/files/ICDC_DGAB_Guidelines_v1.3.pdf</t>
+  </si>
+  <si>
+    <t>(DGAB)</t>
+  </si>
+  <si>
+    <t>https://caninecommons-qa.cancer.gov/#/DGAB</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>https://github.com/CBIIT/icdc-codebase/raw/master/src/main/frontend/src/content/files/ICDC_Data_Submission_Request_Template.docx</t>
+  </si>
+  <si>
+    <t>Data Model Navigator</t>
+  </si>
+  <si>
+    <t>https://caninecommons-qa.cancer.gov/#/icdc-data-model</t>
+  </si>
+  <si>
+    <t>The Integrated Canine Data Commons (ICDC) was established to further research on human cancers by enabling comparative analysis with canine malignancies. Researchers who have data that will contribute to this mission and who are willing to share that data via the ICDC are encouraged to make a data submission request through the Submission Request Process [PDF]. Please email ICDCHelpDesk@mail.nih.gov for specific instructions. All proposed data submissions are reviewed by the Data Governance Advisory Board (DGAB) to assess their scientific value and suitability for inclusion. Once any given study has been fully on-boarded, all data submitted will become publicly available.</t>
+  </si>
+  <si>
+    <t>In support of data submissions, the ICDC application now includes a sophisticated and intuitive Data Model Navigator which provides end users in general, and data submitters in particular, with access to a wealth of information regarding the graph-based data model upon which the ICDC is based.</t>
+  </si>
+  <si>
+    <t>DevelopersDescription1</t>
+  </si>
+  <si>
+    <t>DevelopersDescription2</t>
+  </si>
+  <si>
+    <t>GithubDescription</t>
+  </si>
+  <si>
+    <t>The ICDC has a graph database featuring a read-only GraphQL API based in Java that is available for public consumption and a frontend built from the JavaScript based React library. Each tier in the application stack is designed to be modular and adaptable for a variety of use cases. Users do not require authentication to the system and all data are public.</t>
+  </si>
+  <si>
+    <t>PurposeDescription1</t>
+  </si>
+  <si>
+    <t>PurposeDescription2</t>
+  </si>
+  <si>
+    <t>CrdcLink</t>
+  </si>
+  <si>
+    <t>CloudLink</t>
+  </si>
+  <si>
+    <t>Cancer Research Data Commons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCI's Division of Cancer Treatment and Diagnosis (DCTD) tasked the Frederick National Laboratory for Cancer Research (FNLCR) with building the Integrated Canine Data Commons (ICDC), a cloud-based repository of spontaneously-arising canine cancer data. ICDC was established to further research on human cancers by enabling comparative analysis with canine cancer. The data in the ICDC is sourced from multiple different programs and projects; all focused on canine subjects. The data is harmonized into an integrated data model and then made available to the research community. The ICDC is part of the Cancer Research Data Commons, an initiative from NCI’s Center for Biomedical Informatics and Information Technology (CBIIT). Bioinformatic analysis of the ICDC data is accomplished using the CRDC’s Cloud Resources.
+</t>
+  </si>
+  <si>
+    <t>CommitteeDescription1</t>
+  </si>
+  <si>
+    <t>CommitteeDescription2</t>
+  </si>
+  <si>
+    <t>The Integrated Canine Data Commons (ICDC) is community-driven and built with input and collaboration from many groups to foster a diversity of ideas and to ensure needs are identified across the broad research community. To achieve this collaboration, the ICDC Steering Committee was formed to advise the NCI and FNLCR on the ICDC. The Steering Committee is composed of members from the non-NIH research community, NCI, NHGRI, and NCATS. There is also ex-officio members who are FNLCR staff. All chairpersons are from the non-NIH research community.</t>
+  </si>
+  <si>
+    <t>The Steering Committee has two sub-committees: the Data Governance Advisory Board (DGAB) and the Best Practices Sub-Committee (BPSC).</t>
+  </si>
+  <si>
+    <t>Data Governance Advisory Board</t>
+  </si>
+  <si>
+    <t>Best Practices Sub-Committee</t>
+  </si>
+  <si>
+    <t>PracticesLink</t>
+  </si>
+  <si>
+    <t>DgabLink</t>
+  </si>
+  <si>
+    <t>https://caninecommons-qa.cancer.gov/#/dgab</t>
+  </si>
+  <si>
+    <t>https://caninecommons-qa.cancer.gov/#/bpsc</t>
+  </si>
+  <si>
+    <t>Based upon recommendations from the DGAB, the NCI Senior Advisory Committee (SAC) subsequently makes all final decisions as to the approval and prioritization of incoming studies, including any re-prioritization that may become necessary. The individual members of the SAC are identified below.</t>
+  </si>
+  <si>
+    <t>Data Submission Request Process [PDF]</t>
+  </si>
+  <si>
+    <t>DgabDescription1</t>
+  </si>
+  <si>
+    <t>DgabDescription2</t>
+  </si>
+  <si>
+    <t>SubmissionLink</t>
+  </si>
+  <si>
+    <t>GuidelinesLink</t>
+  </si>
+  <si>
+    <t>Data Submission Guidelines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Integrated Canine Data Commons (ICDC) was established to further research on human cancers by enabling comparative analysis with canine malignancies. Researchers willing to contribute and share relevant data to this mission via the ICDC are encouraged to make a data submission request through the Data Submission Request Process [PDF], and per our Data Submission Guidelines. The request will be processed by ICDC’s Data Governance Advisory Board (DGAB) which consists of 4 external members (all members of the ICDC Steering Committee, with one of the four acting as the DGAB Chair), 2 NIH members, and supported by FNLCR staff. The DGAB meets regularly to prioritize data submission requests and to advise the NCI on the suitability of each proposed data submission for its inclusion in the ICDC. The individual members of the DGAB are identified below.
+</t>
+  </si>
+  <si>
+    <t>Best Practices Subcommittee</t>
+  </si>
+  <si>
+    <t>The Best Practices Subcommittee (BPSC) is responsible for examining completed and planned studies to identify and recommend best practices that the Integrated Canine Data Commons (ICDC) will implement to streamline and harmonize data collection, standardize data formats and platforms, and manage and annotate data (especially clinical data). Moreover, these recommendations will help the broader community in study design and data collection to enhance research to better enable human and canine data comparison. The BPSC is composed of 8 external members, 5 NCI staff, 1 NHGRI staff, and is supported by FNLCR staff.</t>
+  </si>
+  <si>
+    <t>A manuscript from the ICDC BPSC was published by the Journal of Veterinary and Comparative Oncology on October 1, 2023, titled Leading the pack, Best practices in comparative canine cancer genomics to inform human oncology.</t>
+  </si>
+  <si>
+    <t>Leading the pack, Best practices in comparative canine cancer genomics to inform human oncology.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/vco.12935</t>
+  </si>
+  <si>
+    <t>ManuscriptLink</t>
+  </si>
+  <si>
+    <t>BpscDescription1</t>
+  </si>
+  <si>
+    <t>BpscDescription2</t>
+  </si>
+  <si>
+    <t>Working Groups</t>
+  </si>
+  <si>
+    <t>WorkingDescription</t>
+  </si>
+  <si>
+    <t>GoalsTitle</t>
+  </si>
+  <si>
+    <t>Working Group Goals</t>
+  </si>
+  <si>
+    <t>The ICDC encompasses many data types and is currently focused into three working groups; Imaging, Genomics, and Longitudinal Data Use and Acquistion.</t>
+  </si>
+  <si>
+    <t>ImagingDescription</t>
+  </si>
+  <si>
+    <t>GenomicsDescription</t>
+  </si>
+  <si>
+    <t>LongitudinalDescription</t>
+  </si>
+  <si>
+    <t>Imaging Working Group To provide the comparative cancer research community with guidelines and best practices for the collection, formatting and reporting of imaging data collected from canine companion animals with naturally-occurring cancers into the Integrated Canine Data Commons (ICDC). Accomplishing this goal will facilitate the utilization and analysis of such data by stakeholders in the cancer research community and advance dog-to-human translational research in the comparative oncology space.</t>
+  </si>
+  <si>
+    <t>Genomics Working Group To provide an overview of next generation sequencing (NGS) study design, assays and analysis approaches (focusing on genomics and transcriptomics) used by diverse canine cancer research teams alongside annotation of validation studies, canine-specific tooling and parameters, identify common data elements across published analyses, establish general principles in canine cancer genomics best practices modeled on human cancer genomics best practice principles; identify gaps in canine cancer genomics best practices and propose solutions.</t>
+  </si>
+  <si>
+    <t>Longitudinal Data Use &amp; Acquistion Working Group (LDAUWG) To survey the landscape of available longitudinal datasets and identify potential collaborators. Scientific questions and use cases will motivate the efforts to acquire this data for ingestion into the ICDC.</t>
+  </si>
+  <si>
+    <t>Cancer Research Data Commons (CRDC) and Analysis</t>
+  </si>
+  <si>
+    <t>CrdcTitle</t>
+  </si>
+  <si>
+    <t>The CRDC</t>
+  </si>
+  <si>
+    <t>CrdcDescription</t>
+  </si>
+  <si>
+    <t>The CRDC Cloud Resources</t>
+  </si>
+  <si>
+    <t>CrdcCloudTitle</t>
+  </si>
+  <si>
+    <t>CrdcCloudDescription1</t>
+  </si>
+  <si>
+    <t>CrdcCloudDescription2</t>
+  </si>
+  <si>
+    <t>CrdcCloudDescription3</t>
+  </si>
+  <si>
+    <t>These cloud-based platforms eliminate the need for researchers to download and store extremely large files by bringing datasets and powerful analysis tools together within the cloud. The Cloud Resources also provide access to on-demand computational capacity for conducting analysis using publicly available best practice tools and pipelines or building new tools and workflows.</t>
+  </si>
+  <si>
+    <t>All three Cloud Resources provide support for data access through a web-based user interface in addition to programmatic access to analytic tools and workflows, and the capability of sharing results with collaborators. Each Cloud Resource is continually developing new functionality to improve the user experience and add new tools for researchers.</t>
+  </si>
+  <si>
+    <t>The Seven Bridges Cancer Genomics Cloud (CGC) is powered by Velsera and hosted on Amazon Web Services (AWS). The CGC has a rich user interface that allows researchers to find data of interest and combine it with their own private data. Data can be analyzed using more than 900 preinstalled, curated bioinformatics tools and workflows. Researchers can also extend the functionality of the platform by adding their own data and tools via an intuitive software development kit (SDK).</t>
+  </si>
+  <si>
+    <t>IsbCgcDescription</t>
+  </si>
+  <si>
+    <t>FirecloudDescription</t>
+  </si>
+  <si>
+    <t>Institute for Systems Biology Cancer Genomics Cloud (ISB-CGC) leverages many aspects of the Google Cloud Platform (GCP) and allows scientists to interactively define and compare cohorts, examine underlying molecular data for specific genes and pathways, and share insights with collaborators. For computational users, application program interfaces (APIs) and GCP resources such as BigQuery and Google Pipeline service allow complex queries from R or Python scripts or Dockerized workflows to run on data available in Google Cloud Storage.</t>
+  </si>
+  <si>
+    <t>Broad Institute Firecloud is an open, standards-based platform powered by Terra for performing production-scale data analysis in the cloud. Built on the Google Cloud Platform (GCP), Firecloud empowers analysts, tool developers, and production managers to run large-scale analysis and to share results with collaborators. Users can upload their own analysis methods and data to workspaces or run the Broad’s best practice tools and pipelines.</t>
+  </si>
+  <si>
+    <t>IcdcCloudTitle</t>
+  </si>
+  <si>
+    <t>From the ICDC to the Cloud Resources</t>
+  </si>
+  <si>
+    <t>IcdcCloudDescription1</t>
+  </si>
+  <si>
+    <t>IcdcCloudDescription2</t>
+  </si>
+  <si>
+    <t>IcdcCloudDescription3</t>
+  </si>
+  <si>
+    <t>IcdcCloudDescription4</t>
+  </si>
+  <si>
+    <t>Currently the ICDC supports analysis via the Seven Bridges Cancer Genomics Cloud powered by Velsera.</t>
+  </si>
+  <si>
+    <t>One of the primary goals of the ICDC data portal is to make data findable, accessible, interoperable, and reusable (FAIR) to lower the barriers for researchers to go from cohort discovery to a meaningful analysis. Researchers can find cases and build cohorts in the ICDC and then send the associated files required for analysis to the My Files Cart page where the list of files is compiled into a File Manifest. The File Manifest is simply a csv file consisting of rich metadata and Data Repository Service (DRS) Unique Resource Identifiers (URIs) for every file object listed. Using the new Export to the CGC button enables the simple and immediate transfer of a File Manifest to the CGC with only a single click. The CGC uses information in the File Manifest to fetch the file from a DRS server and storage buckets located in the cloud. Alternatively, users can download the File Manifest locally and then subsequently upload the File Manifest directly into the CGC to load files into a CGC project.</t>
+  </si>
+  <si>
+    <t>This Cloud Resource analysis model eliminates the need for researchers to download and store extremely large data sets by allowing them to bring analysis tools to the data in the cloud, instead of the traditional process of bringing the data to the tools on local hardware. The Cloud Resources also provide access to on-demand computational capacity to analyze these data, allow users to run best practice tools and pipelines already implemented, and upload their own data or analysis methods to workspaces.</t>
+  </si>
+  <si>
+    <t>CbiitLink</t>
+  </si>
+  <si>
+    <t>CgcLink</t>
+  </si>
+  <si>
+    <t>IsbCgcLink</t>
+  </si>
+  <si>
+    <t>FirecloudLink</t>
+  </si>
+  <si>
+    <t>The Cancer Research Data Commons (CRDC)</t>
+  </si>
+  <si>
+    <t>https://caninecommons-qa.cancer.gov/CRDC)](https://datacommons.cancer.gov/</t>
+  </si>
+  <si>
+    <t>CBIIT</t>
+  </si>
+  <si>
+    <t>https://datascience.cancer.gov/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seven Bridges Cancer Genomics Cloud powered by Velsera </t>
+  </si>
+  <si>
+    <t>http://www.cancergenomicscloud.org/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISB Cancer Genomics Cloud </t>
+  </si>
+  <si>
+    <t>https://isb-cgc.appspot.com/</t>
+  </si>
+  <si>
+    <t>https://firecloud.terra.bio/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broad Firecloud </t>
+  </si>
+  <si>
+    <t>CgcDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cancer Research Data Commons (CRDC) is an initiative from NCI’s Center for Biomedical Informatics &amp; Information Technology (CBIIT). CBIIT’s vision for the project consists of a virtual, expandable infrastructure that provides secure access to many different data types across scientific domains, allowing users to analyze, share, and store results, leveraging the storage, elastic compute, and scalability of the cloud. The ability to combine diverse data types and perform cross-domain analysis of large data sets can lead to new discoveries in cancer prevention, treatment and diagnosis, and supports the goals of precision medicine and the Cancer Moonshot℠.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CRDC has three Cloud Resources (Seven Bridges Cancer Genomics Cloud powered by Velsera ,ISB Cancer Genomics Cloud , Broad Firecloud ), each providing analysis platforms for the community to use when working with data from the CRDC ecosystem.
+</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Please direct questions, comments, or concerns to ICDCHelpDesk@mail.nih.gov.</t>
+  </si>
+  <si>
+    <t>SupportDescription</t>
   </si>
 </sst>
 </file>
@@ -676,7 +965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -705,6 +994,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -928,8 +1220,8 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -968,10 +1260,10 @@
     </row>
     <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>34</v>
@@ -979,10 +1271,10 @@
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>35</v>
@@ -990,10 +1282,10 @@
     </row>
     <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>36</v>
@@ -1001,10 +1293,10 @@
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>37</v>
@@ -1018,7 +1310,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -1199,38 +1491,344 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F0C310-3A63-3341-B231-C7E6EDBC8E1E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="3" max="3" width="82.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB6797D-D2D1-114E-8E0E-38322A0CA0B6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="89.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="84.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A4" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="84" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1" xr:uid="{F6B1BA7A-00D8-5742-956C-C50F7E16730B}"/>
+    <hyperlink ref="C18" r:id="rId2" xr:uid="{3CBF85BF-13CE-A247-AE1B-9471DA949509}"/>
+    <hyperlink ref="C19" r:id="rId3" xr:uid="{C081F229-A27C-3148-95F4-A99090C32708}"/>
+    <hyperlink ref="C20" r:id="rId4" xr:uid="{26C346B2-7637-B340-8228-3AA6A32528F3}"/>
+    <hyperlink ref="C21" r:id="rId5" xr:uid="{87D9C970-37A4-FE46-966F-F3D1FF3DDAD4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20944CDC-80CA-F946-B43A-2A89C63034E5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="63" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1292,7 +1890,7 @@
         <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C5" s="10"/>
     </row>
@@ -1349,7 +1947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E515A5DD-EF89-E043-A31A-B4906283C62C}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1393,7 +1991,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C4" s="10"/>
     </row>
@@ -1438,7 +2036,7 @@
         <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1495,7 +2093,7 @@
         <v>79</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -1516,57 +2114,57 @@
     </row>
     <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1585,17 +2183,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206BA533-C040-B64B-A1D4-10C8CA9857D3}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="88.6640625" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" customWidth="1"/>
+    <col min="2" max="2" width="80.33203125" customWidth="1"/>
+    <col min="3" max="3" width="77.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
@@ -1605,7 +2203,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1624,99 +2222,149 @@
       <c r="B3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="10"/>
+        <v>187</v>
+      </c>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+        <v>105</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="84" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="168" x14ac:dyDescent="0.15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="182" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A15" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+      <c r="A17" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{D689DA51-5738-EC4C-B63B-26B93237334E}"/>
+    <hyperlink ref="C16" r:id="rId2" location="/DGAB" xr:uid="{0A1248FD-C69A-B443-ABE6-F7446D3F8B48}"/>
+    <hyperlink ref="C17" r:id="rId3" xr:uid="{2E27408E-9FC5-2749-BD0E-C4A04945BE00}"/>
+    <hyperlink ref="C18" r:id="rId4" location="/icdc-data-model" xr:uid="{DA107239-1B52-9941-BE85-99DE39648B77}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1726,12 +2374,12 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19" style="7" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="83.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.6640625" customWidth="1"/>
   </cols>
@@ -1752,106 +2400,106 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="112" x14ac:dyDescent="0.15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="56" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>126</v>
+        <v>190</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="70" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>139</v>
-      </c>
       <c r="C8" s="10" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1873,7 +2521,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1896,46 +2544,46 @@
     </row>
     <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="154" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>152</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="98" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>157</v>
+        <v>196</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>49</v>
@@ -1952,36 +2600,234 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42855C9B-E2AD-E044-8FA6-5C20DCF3D602}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="92" customWidth="1"/>
+    <col min="3" max="3" width="65.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" location="/dgab" xr:uid="{C95F3160-C89D-7644-A653-7922E16288CD}"/>
+    <hyperlink ref="C6" r:id="rId2" location="/bpsc" xr:uid="{8BAA3149-9562-414A-BECA-1188C9446A74}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247298C5-CC1B-2643-8298-2A394565EB0D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="86.1640625" customWidth="1"/>
+    <col min="3" max="3" width="79.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{D47CDEE5-0E27-AA44-9619-E5B6F3103680}"/>
+    <hyperlink ref="C6" r:id="rId2" location="/submit" xr:uid="{D7C0A2B8-84B0-A04B-9C49-99AB92DD9EAE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0273E3E3-64BB-3044-B96A-DE7968AFD02C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="81.1640625" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="98" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{B4287675-70F5-134C-8BB2-D8D23EC8E214}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ICDC upgates for the failed test cases
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/ICDC_StaticData.xlsx
+++ b/InputFiles/ICDC/ICDC_StaticData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/ICDC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\ICDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44254749-EC33-5A47-8498-A77C24D2EF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF58061F-A484-43FA-ABD4-7620E44D3207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="2060" windowWidth="33260" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5676" yWindow="1536" windowWidth="16692" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V_HomePage" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <t>EmbargoTitle</t>
   </si>
   <si>
-    <t>The ICDC discourages use of the data to acquire ownership interest in pre-competitive technologies necessary for the development of the field (“research tools”). The ICDC places no restrictions on the use of data to develop downstream technologies that may lead to discoveries that address public needs, especially therapeutics. For further information about the ICDC Intellectual Property policy, please contact us at ICDCHelpDesk@mail.nih.gov</t>
-  </si>
-  <si>
     <t>FAIR Data</t>
   </si>
   <si>
@@ -592,9 +589,6 @@
   </si>
   <si>
     <t>https://caninecommons-qa.cancer.gov/#/icdc-data-model</t>
-  </si>
-  <si>
-    <t>The Integrated Canine Data Commons (ICDC) was established to further research on human cancers by enabling comparative analysis with canine malignancies. Researchers who have data that will contribute to this mission and who are willing to share that data via the ICDC are encouraged to make a data submission request through the Submission Request Process [PDF]. Please email ICDCHelpDesk@mail.nih.gov for specific instructions. All proposed data submissions are reviewed by the Data Governance Advisory Board (DGAB) to assess their scientific value and suitability for inclusion. Once any given study has been fully on-boarded, all data submitted will become publicly available.</t>
   </si>
   <si>
     <t>In support of data submissions, the ICDC application now includes a sophisticated and intuitive Data Model Navigator which provides end users in general, and data submitters in particular, with access to a wealth of information regarding the graph-based data model upon which the ICDC is based.</t>
@@ -878,6 +872,12 @@
   </si>
   <si>
     <t>SupportDescription</t>
+  </si>
+  <si>
+    <t>The ICDC discourages use of the data to acquire ownership interest in pre-competitive technologies necessary for the development of the field (“research tools”). The ICDC places no restrictions on the use of data to develop downstream technologies that may lead to discoveries that address public needs, especially therapeutics. For further information about the ICDC Intellectual Property policy, please contact us at NCICRDC@mail.nih.gov</t>
+  </si>
+  <si>
+    <t>The Integrated Canine Data Commons (ICDC) was established to further research on human cancers by enabling comparative analysis with canine malignancies. Researchers who have data that will contribute to this mission and who are willing to share that data via the ICDC are encouraged to make a data submission request through the Submission Request Process [PDF]. Please email NCICRDC@mail.nih.gov for specific instructions. All proposed data submissions are reviewed by the Data Governance Advisory Board (DGAB) to assess their scientific value and suitability for inclusion. Once any given study has been fully on-boarded, all data submitted will become publicly available.</t>
   </si>
 </sst>
 </file>
@@ -1220,18 +1220,18 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" customWidth="1"/>
     <col min="2" max="2" width="86" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1258,51 +1258,51 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -1310,10 +1310,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="C15" s="13"/>
     </row>
-    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -1486,6 +1486,7 @@
     <hyperlink ref="C7" r:id="rId15" location="/news" xr:uid="{8B0427EA-A354-8540-901B-992BB2323A8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1497,14 +1498,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
-    <col min="3" max="3" width="82.83203125" customWidth="1"/>
+    <col min="3" max="3" width="82.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1515,53 +1516,53 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="84" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -1577,14 +1578,14 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="89.1640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="89.109375" style="6" customWidth="1"/>
     <col min="3" max="3" width="84.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1595,181 +1596,181 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" ht="98" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="56" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="56" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="56" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="132" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="84" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="140" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="B18" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="56" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -1792,14 +1793,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="63" customWidth="1"/>
     <col min="3" max="3" width="63.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1810,21 +1811,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>280</v>
-      </c>
       <c r="B3" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C3" s="8"/>
     </row>
@@ -1841,14 +1842,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="85.33203125" customWidth="1"/>
     <col min="3" max="3" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>54</v>
       </c>
@@ -1876,7 +1877,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -1885,16 +1886,16 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -1903,7 +1904,7 @@
       </c>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>58</v>
       </c>
@@ -1912,7 +1913,7 @@
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>59</v>
       </c>
@@ -1921,7 +1922,7 @@
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -1930,7 +1931,7 @@
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" ht="42" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1947,18 +1948,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E515A5DD-EF89-E043-A31A-B4906283C62C}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="2" max="2" width="88" customWidth="1"/>
     <col min="3" max="3" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1969,7 +1970,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1986,16 +1987,16 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>72</v>
       </c>
@@ -2004,7 +2005,7 @@
       </c>
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>83</v>
       </c>
@@ -2013,158 +2014,158 @@
       </c>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="C7" s="10"/>
     </row>
-    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="56" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="66" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B20" s="3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A20" s="7" t="s">
+      <c r="C20" s="10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B21" s="8" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
+      <c r="C21" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="B22" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
+      <c r="C22" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B23" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="C23" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2185,18 +2186,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206BA533-C040-B64B-A1D4-10C8CA9857D3}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.33203125" customWidth="1"/>
     <col min="2" max="2" width="80.33203125" customWidth="1"/>
     <col min="3" max="3" width="77.6640625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2207,155 +2208,155 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3" ht="112" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:3" ht="84" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="84" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="98" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+      <c r="B11" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+    <row r="13" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="84" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
+    <row r="14" spans="1:3" ht="171.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="182" x14ac:dyDescent="0.15">
-      <c r="A14" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
+      <c r="C17" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="8" t="s">
         <v>185</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2377,14 +2378,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="7" customWidth="1"/>
-    <col min="2" max="2" width="83.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="83.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="58.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2395,111 +2396,111 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="66" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="70" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="C7" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+      <c r="C9" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A11" s="7" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="14" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2524,14 +2525,14 @@
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="73.1640625" customWidth="1"/>
+    <col min="2" max="2" width="73.109375" customWidth="1"/>
     <col min="3" max="3" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2542,48 +2543,48 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="154" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="98" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>49</v>
@@ -2606,14 +2607,14 @@
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="92" customWidth="1"/>
-    <col min="3" max="3" width="65.5" customWidth="1"/>
+    <col min="3" max="3" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2624,7 +2625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2632,43 +2633,43 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="70" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C5" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="C6" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2688,14 +2689,14 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.1640625" customWidth="1"/>
-    <col min="2" max="2" width="86.1640625" customWidth="1"/>
-    <col min="3" max="3" width="79.5" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="86.109375" customWidth="1"/>
+    <col min="3" max="3" width="79.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2706,48 +2707,48 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="140" x14ac:dyDescent="0.15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>215</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>34</v>
@@ -2770,14 +2771,14 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="81.1640625" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" customWidth="1"/>
+    <col min="2" max="2" width="81.109375" customWidth="1"/>
+    <col min="3" max="3" width="76.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -2788,40 +2789,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="98" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C5" s="10" t="s">
         <v>219</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>